<commit_message>
updated RME jackknives and neg eigen
</commit_message>
<xml_diff>
--- a/Clustering/cell_counts.xlsx
+++ b/Clustering/cell_counts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iuliarusu/Documents/Sharpee/Clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374EC247-119D-0148-8841-D9B315CBF6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA67F47-6C60-CA46-A335-681570F9CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{7DC69461-6F67-2D47-B90B-1F5B39FFC387}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7DC69461-6F67-2D47-B90B-1F5B39FFC387}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>cell</t>
   </si>
@@ -69,19 +70,43 @@
   </si>
   <si>
     <t>lamda dimensionality</t>
+  </si>
+  <si>
+    <t>unclustered</t>
+  </si>
+  <si>
+    <t>clustered</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>408.86759179973296,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,8 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5049114-DF44-8246-B6A2-58147ABBB875}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,19 +672,242 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1A62AA-0155-5441-A23B-08BF3403508F}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4.0926299999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4.1119300000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3.9269799999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>1.9966999999999999</v>
+      </c>
+      <c r="F5">
+        <v>1.88625</v>
+      </c>
+      <c r="G5">
+        <v>1.48621</v>
+      </c>
+      <c r="H5">
+        <v>1.32883</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>368.87984146231599</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>353.98983654932601</v>
+      </c>
+      <c r="E6">
+        <v>389.27098478457702</v>
+      </c>
+      <c r="F6">
+        <v>391.06935931543501</v>
+      </c>
+      <c r="G6">
+        <v>383.10808562598402</v>
+      </c>
+      <c r="H6">
+        <v>399.47930661996099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>3.59897</v>
+      </c>
+      <c r="C9">
+        <v>3.0097499999999999</v>
+      </c>
+      <c r="D9">
+        <v>2.89703</v>
+      </c>
+      <c r="E9">
+        <v>3.1478899999999999</v>
+      </c>
+      <c r="F9">
+        <v>2.99823</v>
+      </c>
+      <c r="G9">
+        <v>3.0981999999999998</v>
+      </c>
+      <c r="H9">
+        <v>3.3106100000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2.6444200000000002</v>
+      </c>
+      <c r="C11">
+        <v>2.4412199999999999</v>
+      </c>
+      <c r="D11">
+        <v>2.1195300000000001</v>
+      </c>
+      <c r="E11">
+        <v>3.2202000000000002</v>
+      </c>
+      <c r="F11">
+        <v>2.0309699999999999</v>
+      </c>
+      <c r="G11">
+        <v>2.44319</v>
+      </c>
+      <c r="H11">
+        <v>2.59429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added plotting functions, latency v radius, pca update, buffer analysis
</commit_message>
<xml_diff>
--- a/Clustering/cell_counts.xlsx
+++ b/Clustering/cell_counts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iuliarusu/Documents/Sharpee/Clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA67F47-6C60-CA46-A335-681570F9CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C2CD31-D1F5-8949-9CAC-955172F801C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7DC69461-6F67-2D47-B90B-1F5B39FFC387}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>cell</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>408.86759179973296,</t>
+  </si>
+  <si>
+    <t>cell_count</t>
   </si>
 </sst>
 </file>
@@ -679,10 +682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1A62AA-0155-5441-A23B-08BF3403508F}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,6 +804,11 @@
         <v>399.47930661996099</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
@@ -908,6 +916,32 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>